<commit_message>
commit final da 2ªfase.
</commit_message>
<xml_diff>
--- a/Schema News.xlsx
+++ b/Schema News.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>NewsReceiver</t>
   </si>
@@ -52,6 +53,15 @@
   <si>
     <t>HttpRequestsToThoth</t>
   </si>
+  <si>
+    <t>thothClasses</t>
+  </si>
+  <si>
+    <t>thothNews</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
 </sst>
 </file>
 
@@ -74,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -144,11 +154,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -160,9 +302,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -183,6 +322,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,6 +1190,506 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="4914900"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" u="sng"/>
+            <a:t>_classId</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="5905500"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>fullname</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3924300" y="6915150"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>showNews</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9048750" y="4962525"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" u="sng"/>
+            <a:t>_classId</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9058275" y="5514975"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>title</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9048750" y="6124575"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>_when</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Oval 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="4914900"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" u="sng"/>
+            <a:t>_newsId</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Oval 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077325" y="6705600"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>content</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Oval 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="6905625"/>
+          <a:ext cx="1143000" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100"/>
+            <a:t>isViewed</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1297,21 +1960,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K36" sqref="K35:L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
@@ -1335,18 +1998,18 @@
         <v>2</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="3"/>
       <c r="H9" s="4"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="11"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1379,18 +2042,129 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="G8:H9"/>
+    <mergeCell ref="G12:H13"/>
     <mergeCell ref="M12:N13"/>
     <mergeCell ref="J4:K5"/>
     <mergeCell ref="D12:E13"/>
     <mergeCell ref="J8:L9"/>
     <mergeCell ref="A12:B13"/>
     <mergeCell ref="G4:H5"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="G8:H9"/>
-    <mergeCell ref="G12:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="J5" s="27"/>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="21"/>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="H9:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>